<commit_message>
post lab meeting update
</commit_message>
<xml_diff>
--- a/analyses/input/Species Traits.xlsx
+++ b/analyses/input/Species Traits.xlsx
@@ -11,7 +11,7 @@
     <sheet name="metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$V$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -1422,7 +1422,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G47" sqref="G47"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1518,22 +1518,22 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="H2" t="s">
         <v>82</v>
       </c>
       <c r="J2" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
@@ -1545,19 +1545,19 @@
         <v>84</v>
       </c>
       <c r="N2" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="O2" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="Q2" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="S2" t="s">
         <v>86</v>
       </c>
       <c r="T2" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="U2" t="b">
         <v>0</v>
@@ -1568,22 +1568,22 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="G3" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="H3" t="s">
         <v>82</v>
       </c>
       <c r="J3" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
@@ -1595,19 +1595,19 @@
         <v>84</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="O3" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="Q3" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="S3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="T3" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="U3" t="b">
         <v>0</v>
@@ -1618,22 +1618,25 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="G4" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="H4" t="s">
         <v>82</v>
       </c>
       <c r="J4" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
@@ -1645,19 +1648,19 @@
         <v>84</v>
       </c>
       <c r="N4" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="O4" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="Q4" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="S4" t="s">
-        <v>91</v>
+        <v>165</v>
       </c>
       <c r="T4" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="U4" t="b">
         <v>0</v>
@@ -1668,19 +1671,25 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>171</v>
       </c>
       <c r="H5" t="s">
         <v>82</v>
       </c>
       <c r="J5" t="s">
-        <v>93</v>
+        <v>172</v>
       </c>
       <c r="K5" t="b">
         <v>1</v>
@@ -1692,19 +1701,19 @@
         <v>84</v>
       </c>
       <c r="N5" t="s">
-        <v>85</v>
+        <v>173</v>
       </c>
       <c r="O5" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="Q5" t="s">
-        <v>92</v>
+        <v>171</v>
       </c>
       <c r="S5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="T5" t="s">
-        <v>93</v>
+        <v>172</v>
       </c>
       <c r="U5" t="b">
         <v>0</v>
@@ -1715,22 +1724,22 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
       <c r="F6" t="s">
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
+        <v>191</v>
       </c>
       <c r="H6" t="s">
         <v>82</v>
       </c>
       <c r="J6" t="s">
-        <v>97</v>
+        <v>192</v>
       </c>
       <c r="K6" t="b">
         <v>1</v>
@@ -1742,19 +1751,19 @@
         <v>84</v>
       </c>
       <c r="N6" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="O6" t="s">
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="Q6" t="s">
-        <v>96</v>
+        <v>191</v>
       </c>
       <c r="S6" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="T6" t="s">
-        <v>97</v>
+        <v>192</v>
       </c>
       <c r="U6" t="b">
         <v>0</v>
@@ -1765,25 +1774,22 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="G7" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
-      </c>
-      <c r="I7" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="J7" t="s">
-        <v>102</v>
+        <v>194</v>
       </c>
       <c r="K7" t="b">
         <v>1</v>
@@ -1795,22 +1801,19 @@
         <v>84</v>
       </c>
       <c r="N7" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="O7" t="s">
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="Q7" t="s">
-        <v>96</v>
-      </c>
-      <c r="R7" t="s">
-        <v>101</v>
+        <v>193</v>
       </c>
       <c r="S7" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="T7" t="s">
-        <v>102</v>
+        <v>194</v>
       </c>
       <c r="U7" t="b">
         <v>0</v>
@@ -1821,22 +1824,22 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>104</v>
+        <v>190</v>
       </c>
       <c r="G8" t="s">
-        <v>105</v>
+        <v>195</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
       </c>
       <c r="J8" t="s">
-        <v>106</v>
+        <v>196</v>
       </c>
       <c r="K8" t="b">
         <v>1</v>
@@ -1848,19 +1851,19 @@
         <v>84</v>
       </c>
       <c r="N8" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="O8" t="s">
-        <v>104</v>
+        <v>190</v>
       </c>
       <c r="Q8" t="s">
-        <v>105</v>
+        <v>195</v>
       </c>
       <c r="S8" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="T8" t="s">
-        <v>106</v>
+        <v>196</v>
       </c>
       <c r="U8" t="b">
         <v>0</v>
@@ -1871,22 +1874,22 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>104</v>
+        <v>237</v>
       </c>
       <c r="G9" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="H9" t="s">
         <v>82</v>
       </c>
       <c r="J9" t="s">
-        <v>110</v>
+        <v>238</v>
       </c>
       <c r="K9" t="b">
         <v>1</v>
@@ -1898,19 +1901,19 @@
         <v>84</v>
       </c>
       <c r="N9" t="s">
-        <v>107</v>
+        <v>239</v>
       </c>
       <c r="O9" t="s">
-        <v>104</v>
+        <v>237</v>
       </c>
       <c r="Q9" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="S9" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="T9" t="s">
-        <v>110</v>
+        <v>238</v>
       </c>
       <c r="U9" t="b">
         <v>0</v>
@@ -1921,22 +1924,28 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>112</v>
+        <v>248</v>
       </c>
       <c r="G10" t="s">
-        <v>113</v>
+        <v>249</v>
       </c>
       <c r="H10" t="s">
         <v>82</v>
       </c>
       <c r="J10" t="s">
-        <v>114</v>
+        <v>250</v>
       </c>
       <c r="K10" t="b">
         <v>1</v>
@@ -1945,22 +1954,22 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M10" t="s">
-        <v>84</v>
+        <v>200</v>
       </c>
       <c r="N10" t="s">
-        <v>107</v>
+        <v>251</v>
       </c>
       <c r="O10" t="s">
-        <v>112</v>
+        <v>248</v>
       </c>
       <c r="Q10" t="s">
-        <v>113</v>
+        <v>252</v>
       </c>
       <c r="S10" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="T10" t="s">
-        <v>114</v>
+        <v>253</v>
       </c>
       <c r="U10" t="b">
         <v>0</v>
@@ -1971,22 +1980,25 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="G11" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="H11" t="s">
         <v>82</v>
       </c>
       <c r="J11" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="K11" t="b">
         <v>1</v>
@@ -1998,19 +2010,19 @@
         <v>84</v>
       </c>
       <c r="N11" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="O11" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="Q11" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="S11" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="T11" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="U11" t="b">
         <v>0</v>
@@ -2021,22 +2033,22 @@
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="G12" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="H12" t="s">
         <v>82</v>
       </c>
       <c r="J12" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
       <c r="K12" t="b">
         <v>1</v>
@@ -2048,19 +2060,19 @@
         <v>84</v>
       </c>
       <c r="N12" t="s">
-        <v>98</v>
+        <v>157</v>
       </c>
       <c r="O12" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="Q12" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="S12" t="s">
-        <v>86</v>
+        <v>158</v>
       </c>
       <c r="T12" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
       <c r="U12" t="b">
         <v>0</v>
@@ -2071,22 +2083,25 @@
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>254</v>
       </c>
       <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="G13" t="s">
-        <v>122</v>
+        <v>255</v>
       </c>
       <c r="H13" t="s">
         <v>82</v>
       </c>
       <c r="J13" t="s">
-        <v>123</v>
+        <v>256</v>
       </c>
       <c r="K13" t="b">
         <v>1</v>
@@ -2098,19 +2113,19 @@
         <v>84</v>
       </c>
       <c r="N13" t="s">
-        <v>98</v>
+        <v>157</v>
       </c>
       <c r="O13" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="Q13" t="s">
-        <v>122</v>
+        <v>255</v>
       </c>
       <c r="S13" t="s">
-        <v>91</v>
+        <v>257</v>
       </c>
       <c r="T13" t="s">
-        <v>123</v>
+        <v>256</v>
       </c>
       <c r="U13" t="b">
         <v>0</v>
@@ -2121,22 +2136,28 @@
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
         <v>5</v>
       </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
       <c r="F14" t="s">
-        <v>116</v>
+        <v>180</v>
       </c>
       <c r="G14" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="H14" t="s">
         <v>82</v>
       </c>
       <c r="J14" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="K14" t="b">
         <v>1</v>
@@ -2148,19 +2169,19 @@
         <v>84</v>
       </c>
       <c r="N14" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
       <c r="O14" t="s">
-        <v>116</v>
+        <v>180</v>
       </c>
       <c r="Q14" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="S14" t="s">
-        <v>91</v>
+        <v>184</v>
       </c>
       <c r="T14" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="U14" t="b">
         <v>0</v>
@@ -2171,25 +2192,28 @@
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F15" t="s">
-        <v>126</v>
+        <v>180</v>
       </c>
       <c r="G15" t="s">
-        <v>127</v>
+        <v>185</v>
       </c>
       <c r="H15" t="s">
         <v>82</v>
       </c>
       <c r="J15" t="s">
-        <v>128</v>
+        <v>186</v>
       </c>
       <c r="K15" t="b">
         <v>1</v>
@@ -2201,19 +2225,19 @@
         <v>84</v>
       </c>
       <c r="N15" t="s">
-        <v>129</v>
+        <v>183</v>
       </c>
       <c r="O15" t="s">
-        <v>126</v>
+        <v>180</v>
       </c>
       <c r="Q15" t="s">
-        <v>127</v>
+        <v>185</v>
       </c>
       <c r="S15" t="s">
-        <v>130</v>
+        <v>184</v>
       </c>
       <c r="T15" t="s">
-        <v>128</v>
+        <v>186</v>
       </c>
       <c r="U15" t="b">
         <v>0</v>
@@ -2223,23 +2247,29 @@
       </c>
     </row>
     <row r="16" spans="1:22">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
+      <c r="A16" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
         <v>5</v>
       </c>
+      <c r="D16" t="s">
+        <v>258</v>
+      </c>
       <c r="F16" t="s">
-        <v>131</v>
+        <v>197</v>
       </c>
       <c r="G16" t="s">
-        <v>132</v>
+        <v>198</v>
       </c>
       <c r="H16" t="s">
         <v>82</v>
       </c>
       <c r="J16" t="s">
-        <v>133</v>
+        <v>199</v>
       </c>
       <c r="K16" t="b">
         <v>1</v>
@@ -2248,22 +2278,22 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M16" t="s">
-        <v>84</v>
+        <v>200</v>
       </c>
       <c r="N16" t="s">
-        <v>98</v>
+        <v>201</v>
       </c>
       <c r="O16" t="s">
-        <v>131</v>
+        <v>202</v>
       </c>
       <c r="Q16" t="s">
-        <v>132</v>
+        <v>203</v>
       </c>
       <c r="S16" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="T16" t="s">
-        <v>133</v>
+        <v>204</v>
       </c>
       <c r="U16" t="b">
         <v>0</v>
@@ -2274,19 +2304,28 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
       </c>
       <c r="F17" t="s">
-        <v>134</v>
+        <v>209</v>
       </c>
       <c r="G17" t="s">
-        <v>135</v>
+        <v>210</v>
       </c>
       <c r="H17" t="s">
         <v>82</v>
       </c>
       <c r="J17" t="s">
-        <v>136</v>
+        <v>211</v>
       </c>
       <c r="K17" t="b">
         <v>1</v>
@@ -2298,19 +2337,19 @@
         <v>84</v>
       </c>
       <c r="N17" t="s">
-        <v>137</v>
+        <v>212</v>
       </c>
       <c r="O17" t="s">
-        <v>134</v>
+        <v>209</v>
       </c>
       <c r="Q17" t="s">
-        <v>135</v>
+        <v>210</v>
       </c>
       <c r="S17" t="s">
-        <v>138</v>
+        <v>213</v>
       </c>
       <c r="T17" t="s">
-        <v>136</v>
+        <v>211</v>
       </c>
       <c r="U17" t="b">
         <v>0</v>
@@ -2321,7 +2360,7 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -2330,16 +2369,16 @@
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>139</v>
+        <v>214</v>
       </c>
       <c r="G18" t="s">
-        <v>140</v>
+        <v>221</v>
       </c>
       <c r="H18" t="s">
         <v>82</v>
       </c>
       <c r="J18" t="s">
-        <v>141</v>
+        <v>222</v>
       </c>
       <c r="K18" t="b">
         <v>1</v>
@@ -2351,19 +2390,19 @@
         <v>84</v>
       </c>
       <c r="N18" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="O18" t="s">
-        <v>139</v>
+        <v>214</v>
       </c>
       <c r="Q18" t="s">
-        <v>140</v>
+        <v>221</v>
       </c>
       <c r="S18" t="s">
-        <v>143</v>
+        <v>220</v>
       </c>
       <c r="T18" t="s">
-        <v>141</v>
+        <v>222</v>
       </c>
       <c r="U18" t="b">
         <v>0</v>
@@ -2374,13 +2413,16 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>144</v>
+        <v>227</v>
       </c>
       <c r="G19" t="s">
         <v>145</v>
@@ -2389,7 +2431,7 @@
         <v>82</v>
       </c>
       <c r="J19" t="s">
-        <v>146</v>
+        <v>228</v>
       </c>
       <c r="K19" t="b">
         <v>1</v>
@@ -2401,19 +2443,19 @@
         <v>84</v>
       </c>
       <c r="N19" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="O19" t="s">
-        <v>144</v>
+        <v>227</v>
       </c>
       <c r="Q19" t="s">
         <v>145</v>
       </c>
       <c r="S19" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="T19" t="s">
-        <v>146</v>
+        <v>228</v>
       </c>
       <c r="U19" t="b">
         <v>0</v>
@@ -2424,22 +2466,28 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
       </c>
       <c r="F20" t="s">
-        <v>144</v>
+        <v>229</v>
       </c>
       <c r="G20" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="H20" t="s">
         <v>82</v>
       </c>
       <c r="J20" t="s">
-        <v>149</v>
+        <v>230</v>
       </c>
       <c r="K20" t="b">
         <v>1</v>
@@ -2451,19 +2499,19 @@
         <v>84</v>
       </c>
       <c r="N20" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="O20" t="s">
-        <v>144</v>
+        <v>229</v>
       </c>
       <c r="Q20" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="S20" t="s">
-        <v>91</v>
+        <v>231</v>
       </c>
       <c r="T20" t="s">
-        <v>149</v>
+        <v>230</v>
       </c>
       <c r="U20" t="b">
         <v>0</v>
@@ -2474,22 +2522,28 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
         <v>5</v>
       </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
       <c r="F21" t="s">
-        <v>150</v>
+        <v>229</v>
       </c>
       <c r="G21" t="s">
-        <v>151</v>
+        <v>232</v>
       </c>
       <c r="H21" t="s">
         <v>82</v>
       </c>
       <c r="J21" t="s">
-        <v>152</v>
+        <v>233</v>
       </c>
       <c r="K21" t="b">
         <v>1</v>
@@ -2501,19 +2555,19 @@
         <v>84</v>
       </c>
       <c r="N21" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="O21" t="s">
-        <v>150</v>
+        <v>229</v>
       </c>
       <c r="Q21" t="s">
-        <v>151</v>
+        <v>232</v>
       </c>
       <c r="S21" t="s">
         <v>86</v>
       </c>
       <c r="T21" t="s">
-        <v>152</v>
+        <v>233</v>
       </c>
       <c r="U21" t="b">
         <v>0</v>
@@ -2524,22 +2578,28 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
       <c r="F22" t="s">
-        <v>154</v>
+        <v>243</v>
       </c>
       <c r="G22" t="s">
-        <v>155</v>
+        <v>244</v>
       </c>
       <c r="H22" t="s">
         <v>82</v>
       </c>
       <c r="J22" t="s">
-        <v>156</v>
+        <v>245</v>
       </c>
       <c r="K22" t="b">
         <v>1</v>
@@ -2551,19 +2611,19 @@
         <v>84</v>
       </c>
       <c r="N22" t="s">
-        <v>157</v>
+        <v>226</v>
       </c>
       <c r="O22" t="s">
-        <v>154</v>
+        <v>243</v>
       </c>
       <c r="Q22" t="s">
-        <v>155</v>
+        <v>244</v>
       </c>
       <c r="S22" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="T22" t="s">
-        <v>156</v>
+        <v>245</v>
       </c>
       <c r="U22" t="b">
         <v>0</v>
@@ -2574,7 +2634,7 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="1" t="s">
-        <v>254</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -2583,16 +2643,16 @@
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>154</v>
+        <v>243</v>
       </c>
       <c r="G23" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="H23" t="s">
         <v>82</v>
       </c>
       <c r="J23" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="K23" t="b">
         <v>1</v>
@@ -2604,19 +2664,19 @@
         <v>84</v>
       </c>
       <c r="N23" t="s">
-        <v>157</v>
+        <v>226</v>
       </c>
       <c r="O23" t="s">
-        <v>154</v>
+        <v>243</v>
       </c>
       <c r="Q23" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="S23" t="s">
-        <v>257</v>
+        <v>184</v>
       </c>
       <c r="T23" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="U23" t="b">
         <v>0</v>
@@ -2627,22 +2687,22 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B24">
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>159</v>
+        <v>80</v>
       </c>
       <c r="G24" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
       <c r="H24" t="s">
         <v>82</v>
       </c>
       <c r="J24" t="s">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="K24" t="b">
         <v>1</v>
@@ -2654,19 +2714,19 @@
         <v>84</v>
       </c>
       <c r="N24" t="s">
-        <v>162</v>
+        <v>85</v>
       </c>
       <c r="O24" t="s">
-        <v>159</v>
+        <v>80</v>
       </c>
       <c r="Q24" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
       <c r="S24" t="s">
         <v>86</v>
       </c>
       <c r="T24" t="s">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="U24" t="b">
         <v>0</v>
@@ -2677,25 +2737,22 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B25">
-        <v>3</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>163</v>
+        <v>80</v>
       </c>
       <c r="G25" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="H25" t="s">
         <v>82</v>
       </c>
       <c r="J25" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
       <c r="K25" t="b">
         <v>1</v>
@@ -2707,19 +2764,19 @@
         <v>84</v>
       </c>
       <c r="N25" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="O25" t="s">
-        <v>163</v>
+        <v>80</v>
       </c>
       <c r="Q25" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="S25" t="s">
-        <v>165</v>
+        <v>86</v>
       </c>
       <c r="T25" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
       <c r="U25" t="b">
         <v>0</v>
@@ -2730,22 +2787,22 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" t="s">
-        <v>60</v>
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>166</v>
+        <v>80</v>
       </c>
       <c r="G26" t="s">
-        <v>167</v>
+        <v>89</v>
       </c>
       <c r="H26" t="s">
         <v>82</v>
       </c>
       <c r="J26" t="s">
-        <v>168</v>
+        <v>90</v>
       </c>
       <c r="K26" t="b">
         <v>1</v>
@@ -2757,19 +2814,19 @@
         <v>84</v>
       </c>
       <c r="N26" t="s">
-        <v>162</v>
+        <v>85</v>
       </c>
       <c r="O26" t="s">
-        <v>166</v>
+        <v>80</v>
       </c>
       <c r="Q26" t="s">
-        <v>167</v>
+        <v>89</v>
       </c>
       <c r="S26" t="s">
-        <v>169</v>
+        <v>91</v>
       </c>
       <c r="T26" t="s">
-        <v>168</v>
+        <v>90</v>
       </c>
       <c r="U26" t="b">
         <v>0</v>
@@ -2780,25 +2837,22 @@
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>170</v>
+        <v>95</v>
       </c>
       <c r="G27" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="H27" t="s">
         <v>82</v>
       </c>
       <c r="J27" t="s">
-        <v>172</v>
+        <v>97</v>
       </c>
       <c r="K27" t="b">
         <v>1</v>
@@ -2810,19 +2864,19 @@
         <v>84</v>
       </c>
       <c r="N27" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="O27" t="s">
-        <v>170</v>
+        <v>95</v>
       </c>
       <c r="Q27" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="S27" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="T27" t="s">
-        <v>172</v>
+        <v>97</v>
       </c>
       <c r="U27" t="b">
         <v>0</v>
@@ -2833,25 +2887,25 @@
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B28">
         <v>5</v>
       </c>
-      <c r="D28" t="s">
-        <v>61</v>
-      </c>
       <c r="F28" t="s">
-        <v>174</v>
+        <v>95</v>
       </c>
       <c r="G28" t="s">
-        <v>175</v>
+        <v>96</v>
       </c>
       <c r="H28" t="s">
-        <v>82</v>
+        <v>100</v>
+      </c>
+      <c r="I28" t="s">
+        <v>101</v>
       </c>
       <c r="J28" t="s">
-        <v>176</v>
+        <v>102</v>
       </c>
       <c r="K28" t="b">
         <v>1</v>
@@ -2863,19 +2917,22 @@
         <v>84</v>
       </c>
       <c r="N28" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="O28" t="s">
-        <v>174</v>
+        <v>95</v>
       </c>
       <c r="Q28" t="s">
-        <v>175</v>
+        <v>96</v>
+      </c>
+      <c r="R28" t="s">
+        <v>101</v>
       </c>
       <c r="S28" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="T28" t="s">
-        <v>176</v>
+        <v>102</v>
       </c>
       <c r="U28" t="b">
         <v>0</v>
@@ -2886,22 +2943,22 @@
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>177</v>
+        <v>104</v>
       </c>
       <c r="G29" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="H29" t="s">
         <v>82</v>
       </c>
       <c r="J29" t="s">
-        <v>178</v>
+        <v>106</v>
       </c>
       <c r="K29" t="b">
         <v>1</v>
@@ -2913,19 +2970,19 @@
         <v>84</v>
       </c>
       <c r="N29" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="O29" t="s">
-        <v>177</v>
+        <v>104</v>
       </c>
       <c r="Q29" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="S29" t="s">
-        <v>179</v>
+        <v>108</v>
       </c>
       <c r="T29" t="s">
-        <v>178</v>
+        <v>106</v>
       </c>
       <c r="U29" t="b">
         <v>0</v>
@@ -2936,28 +2993,22 @@
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="C30">
         <v>5</v>
       </c>
-      <c r="D30" t="s">
-        <v>62</v>
-      </c>
       <c r="F30" t="s">
-        <v>180</v>
+        <v>104</v>
       </c>
       <c r="G30" t="s">
-        <v>181</v>
+        <v>109</v>
       </c>
       <c r="H30" t="s">
         <v>82</v>
       </c>
       <c r="J30" t="s">
-        <v>182</v>
+        <v>110</v>
       </c>
       <c r="K30" t="b">
         <v>1</v>
@@ -2969,19 +3020,19 @@
         <v>84</v>
       </c>
       <c r="N30" t="s">
-        <v>183</v>
+        <v>107</v>
       </c>
       <c r="O30" t="s">
-        <v>180</v>
+        <v>104</v>
       </c>
       <c r="Q30" t="s">
-        <v>181</v>
+        <v>109</v>
       </c>
       <c r="S30" t="s">
-        <v>184</v>
+        <v>111</v>
       </c>
       <c r="T30" t="s">
-        <v>182</v>
+        <v>110</v>
       </c>
       <c r="U30" t="b">
         <v>0</v>
@@ -2992,28 +3043,22 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="C31">
         <v>5</v>
       </c>
-      <c r="D31" t="s">
-        <v>61</v>
-      </c>
       <c r="F31" t="s">
-        <v>180</v>
+        <v>112</v>
       </c>
       <c r="G31" t="s">
-        <v>185</v>
+        <v>113</v>
       </c>
       <c r="H31" t="s">
         <v>82</v>
       </c>
       <c r="J31" t="s">
-        <v>186</v>
+        <v>114</v>
       </c>
       <c r="K31" t="b">
         <v>1</v>
@@ -3025,19 +3070,19 @@
         <v>84</v>
       </c>
       <c r="N31" t="s">
-        <v>183</v>
+        <v>107</v>
       </c>
       <c r="O31" t="s">
-        <v>180</v>
+        <v>112</v>
       </c>
       <c r="Q31" t="s">
-        <v>185</v>
+        <v>113</v>
       </c>
       <c r="S31" t="s">
-        <v>184</v>
+        <v>115</v>
       </c>
       <c r="T31" t="s">
-        <v>186</v>
+        <v>114</v>
       </c>
       <c r="U31" t="b">
         <v>0</v>
@@ -3048,28 +3093,22 @@
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B32">
         <v>5</v>
       </c>
-      <c r="C32">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>63</v>
-      </c>
       <c r="F32" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
       <c r="G32" t="s">
-        <v>188</v>
+        <v>117</v>
       </c>
       <c r="H32" t="s">
         <v>82</v>
       </c>
       <c r="J32" t="s">
-        <v>189</v>
+        <v>118</v>
       </c>
       <c r="K32" t="b">
         <v>1</v>
@@ -3081,19 +3120,19 @@
         <v>84</v>
       </c>
       <c r="N32" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="O32" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
       <c r="Q32" t="s">
-        <v>188</v>
+        <v>117</v>
       </c>
       <c r="S32" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="T32" t="s">
-        <v>189</v>
+        <v>118</v>
       </c>
       <c r="U32" t="b">
         <v>0</v>
@@ -3104,22 +3143,22 @@
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F33" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="G33" t="s">
-        <v>191</v>
+        <v>120</v>
       </c>
       <c r="H33" t="s">
         <v>82</v>
       </c>
       <c r="J33" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="K33" t="b">
         <v>1</v>
@@ -3131,19 +3170,19 @@
         <v>84</v>
       </c>
       <c r="N33" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="O33" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="Q33" t="s">
-        <v>191</v>
+        <v>120</v>
       </c>
       <c r="S33" t="s">
         <v>86</v>
       </c>
       <c r="T33" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="U33" t="b">
         <v>0</v>
@@ -3154,22 +3193,22 @@
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F34" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="G34" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="H34" t="s">
         <v>82</v>
       </c>
       <c r="J34" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="K34" t="b">
         <v>1</v>
@@ -3181,19 +3220,19 @@
         <v>84</v>
       </c>
       <c r="N34" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="O34" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="Q34" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="S34" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="T34" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="U34" t="b">
         <v>0</v>
@@ -3204,22 +3243,22 @@
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F35" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="G35" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="H35" t="s">
         <v>82</v>
       </c>
       <c r="J35" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="K35" t="b">
         <v>1</v>
@@ -3231,19 +3270,19 @@
         <v>84</v>
       </c>
       <c r="N35" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="O35" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="Q35" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="S35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T35" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="U35" t="b">
         <v>0</v>
@@ -3253,29 +3292,26 @@
       </c>
     </row>
     <row r="36" spans="1:22">
-      <c r="A36" s="2" t="s">
-        <v>22</v>
+      <c r="A36" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B36">
-        <v>4</v>
-      </c>
-      <c r="C36">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>258</v>
+        <v>64</v>
       </c>
       <c r="F36" t="s">
-        <v>197</v>
+        <v>126</v>
       </c>
       <c r="G36" t="s">
-        <v>198</v>
+        <v>127</v>
       </c>
       <c r="H36" t="s">
         <v>82</v>
       </c>
       <c r="J36" t="s">
-        <v>199</v>
+        <v>128</v>
       </c>
       <c r="K36" t="b">
         <v>1</v>
@@ -3284,22 +3320,22 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M36" t="s">
-        <v>200</v>
+        <v>84</v>
       </c>
       <c r="N36" t="s">
-        <v>201</v>
+        <v>129</v>
       </c>
       <c r="O36" t="s">
-        <v>202</v>
+        <v>126</v>
       </c>
       <c r="Q36" t="s">
-        <v>203</v>
+        <v>127</v>
       </c>
       <c r="S36" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="T36" t="s">
-        <v>204</v>
+        <v>128</v>
       </c>
       <c r="U36" t="b">
         <v>0</v>
@@ -3310,22 +3346,22 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" t="s">
-        <v>65</v>
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
       </c>
       <c r="F37" t="s">
-        <v>205</v>
+        <v>131</v>
       </c>
       <c r="G37" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="H37" t="s">
         <v>82</v>
       </c>
       <c r="J37" t="s">
-        <v>207</v>
+        <v>133</v>
       </c>
       <c r="K37" t="b">
         <v>1</v>
@@ -3337,19 +3373,19 @@
         <v>84</v>
       </c>
       <c r="N37" t="s">
-        <v>162</v>
+        <v>98</v>
       </c>
       <c r="O37" t="s">
-        <v>205</v>
+        <v>131</v>
       </c>
       <c r="Q37" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="S37" t="s">
-        <v>208</v>
+        <v>91</v>
       </c>
       <c r="T37" t="s">
-        <v>207</v>
+        <v>133</v>
       </c>
       <c r="U37" t="b">
         <v>0</v>
@@ -3360,28 +3396,22 @@
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="1" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B38">
-        <v>4</v>
-      </c>
-      <c r="C38">
         <v>5</v>
       </c>
-      <c r="D38" t="s">
-        <v>61</v>
-      </c>
       <c r="F38" t="s">
-        <v>209</v>
+        <v>150</v>
       </c>
       <c r="G38" t="s">
-        <v>210</v>
+        <v>151</v>
       </c>
       <c r="H38" t="s">
         <v>82</v>
       </c>
       <c r="J38" t="s">
-        <v>211</v>
+        <v>152</v>
       </c>
       <c r="K38" t="b">
         <v>1</v>
@@ -3393,19 +3423,19 @@
         <v>84</v>
       </c>
       <c r="N38" t="s">
-        <v>212</v>
+        <v>153</v>
       </c>
       <c r="O38" t="s">
-        <v>209</v>
+        <v>150</v>
       </c>
       <c r="Q38" t="s">
-        <v>210</v>
+        <v>151</v>
       </c>
       <c r="S38" t="s">
-        <v>213</v>
+        <v>86</v>
       </c>
       <c r="T38" t="s">
-        <v>211</v>
+        <v>152</v>
       </c>
       <c r="U38" t="b">
         <v>0</v>
@@ -3416,28 +3446,22 @@
     </row>
     <row r="39" spans="1:22">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B39">
         <v>5</v>
       </c>
-      <c r="C39">
-        <v>4</v>
-      </c>
-      <c r="D39" t="s">
-        <v>61</v>
-      </c>
       <c r="F39" t="s">
-        <v>214</v>
+        <v>159</v>
       </c>
       <c r="G39" t="s">
-        <v>215</v>
+        <v>160</v>
       </c>
       <c r="H39" t="s">
         <v>82</v>
       </c>
       <c r="J39" t="s">
-        <v>216</v>
+        <v>161</v>
       </c>
       <c r="K39" t="b">
         <v>1</v>
@@ -3449,19 +3473,19 @@
         <v>84</v>
       </c>
       <c r="N39" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="O39" t="s">
-        <v>214</v>
+        <v>159</v>
       </c>
       <c r="Q39" t="s">
-        <v>215</v>
+        <v>160</v>
       </c>
       <c r="S39" t="s">
-        <v>217</v>
+        <v>86</v>
       </c>
       <c r="T39" t="s">
-        <v>216</v>
+        <v>161</v>
       </c>
       <c r="U39" t="b">
         <v>0</v>
@@ -3472,25 +3496,25 @@
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B40">
         <v>5</v>
       </c>
-      <c r="C40">
-        <v>4</v>
+      <c r="D40" t="s">
+        <v>61</v>
       </c>
       <c r="F40" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="G40" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="H40" t="s">
         <v>82</v>
       </c>
       <c r="J40" t="s">
-        <v>219</v>
+        <v>176</v>
       </c>
       <c r="K40" t="b">
         <v>1</v>
@@ -3502,19 +3526,19 @@
         <v>84</v>
       </c>
       <c r="N40" t="s">
-        <v>183</v>
+        <v>129</v>
       </c>
       <c r="O40" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="Q40" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="S40" t="s">
-        <v>220</v>
+        <v>91</v>
       </c>
       <c r="T40" t="s">
-        <v>219</v>
+        <v>176</v>
       </c>
       <c r="U40" t="b">
         <v>0</v>
@@ -3525,25 +3549,22 @@
     </row>
     <row r="41" spans="1:22">
       <c r="A41" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B41">
-        <v>4</v>
-      </c>
-      <c r="C41">
         <v>5</v>
       </c>
       <c r="F41" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="G41" t="s">
-        <v>221</v>
+        <v>151</v>
       </c>
       <c r="H41" t="s">
         <v>82</v>
       </c>
       <c r="J41" t="s">
-        <v>222</v>
+        <v>178</v>
       </c>
       <c r="K41" t="b">
         <v>1</v>
@@ -3555,19 +3576,19 @@
         <v>84</v>
       </c>
       <c r="N41" t="s">
-        <v>183</v>
+        <v>98</v>
       </c>
       <c r="O41" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="Q41" t="s">
-        <v>221</v>
+        <v>151</v>
       </c>
       <c r="S41" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="T41" t="s">
-        <v>222</v>
+        <v>178</v>
       </c>
       <c r="U41" t="b">
         <v>0</v>
@@ -3578,22 +3599,28 @@
     </row>
     <row r="42" spans="1:22">
       <c r="A42" s="1" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B42">
         <v>5</v>
       </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
       <c r="F42" t="s">
-        <v>223</v>
+        <v>187</v>
       </c>
       <c r="G42" t="s">
-        <v>224</v>
+        <v>188</v>
       </c>
       <c r="H42" t="s">
         <v>82</v>
       </c>
       <c r="J42" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="K42" t="b">
         <v>1</v>
@@ -3605,19 +3632,19 @@
         <v>84</v>
       </c>
       <c r="N42" t="s">
-        <v>226</v>
+        <v>107</v>
       </c>
       <c r="O42" t="s">
-        <v>223</v>
+        <v>187</v>
       </c>
       <c r="Q42" t="s">
-        <v>224</v>
+        <v>188</v>
       </c>
       <c r="S42" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="T42" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="U42" t="b">
         <v>0</v>
@@ -3628,25 +3655,28 @@
     </row>
     <row r="43" spans="1:22">
       <c r="A43" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43">
         <v>4</v>
       </c>
-      <c r="C43">
-        <v>5</v>
+      <c r="D43" t="s">
+        <v>61</v>
       </c>
       <c r="F43" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="G43" t="s">
-        <v>145</v>
+        <v>215</v>
       </c>
       <c r="H43" t="s">
         <v>82</v>
       </c>
       <c r="J43" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="K43" t="b">
         <v>1</v>
@@ -3658,19 +3688,19 @@
         <v>84</v>
       </c>
       <c r="N43" t="s">
-        <v>107</v>
+        <v>183</v>
       </c>
       <c r="O43" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="Q43" t="s">
-        <v>145</v>
+        <v>215</v>
       </c>
       <c r="S43" t="s">
-        <v>91</v>
+        <v>217</v>
       </c>
       <c r="T43" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="U43" t="b">
         <v>0</v>
@@ -3681,28 +3711,25 @@
     </row>
     <row r="44" spans="1:22">
       <c r="A44" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
         <v>4</v>
       </c>
-      <c r="C44">
-        <v>5</v>
-      </c>
-      <c r="D44" t="s">
-        <v>64</v>
-      </c>
       <c r="F44" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="G44" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="H44" t="s">
         <v>82</v>
       </c>
       <c r="J44" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="K44" t="b">
         <v>1</v>
@@ -3714,19 +3741,19 @@
         <v>84</v>
       </c>
       <c r="N44" t="s">
-        <v>107</v>
+        <v>183</v>
       </c>
       <c r="O44" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="Q44" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="S44" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="T44" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="U44" t="b">
         <v>0</v>
@@ -3737,28 +3764,22 @@
     </row>
     <row r="45" spans="1:22">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B45">
-        <v>4</v>
-      </c>
-      <c r="C45">
         <v>5</v>
       </c>
-      <c r="D45" t="s">
-        <v>64</v>
-      </c>
       <c r="F45" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G45" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="H45" t="s">
         <v>82</v>
       </c>
       <c r="J45" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="K45" t="b">
         <v>1</v>
@@ -3770,19 +3791,19 @@
         <v>84</v>
       </c>
       <c r="N45" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="O45" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="Q45" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="S45" t="s">
         <v>86</v>
       </c>
       <c r="T45" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="U45" t="b">
         <v>0</v>
@@ -3842,23 +3863,26 @@
       </c>
     </row>
     <row r="47" spans="1:22">
-      <c r="A47" s="1" t="s">
-        <v>47</v>
+      <c r="A47" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>61</v>
       </c>
       <c r="F47" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G47" t="s">
-        <v>145</v>
+        <v>241</v>
       </c>
       <c r="H47" t="s">
         <v>82</v>
       </c>
       <c r="J47" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="K47" t="b">
         <v>1</v>
@@ -3870,19 +3894,19 @@
         <v>84</v>
       </c>
       <c r="N47" t="s">
-        <v>239</v>
+        <v>162</v>
       </c>
       <c r="O47" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="Q47" t="s">
-        <v>145</v>
+        <v>241</v>
       </c>
       <c r="S47" t="s">
-        <v>86</v>
+        <v>184</v>
       </c>
       <c r="T47" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="U47" t="b">
         <v>0</v>
@@ -3892,26 +3916,20 @@
       </c>
     </row>
     <row r="48" spans="1:22">
-      <c r="A48" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48">
-        <v>5</v>
-      </c>
-      <c r="D48" t="s">
-        <v>61</v>
+      <c r="A48" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="F48" t="s">
-        <v>240</v>
+        <v>80</v>
       </c>
       <c r="G48" t="s">
-        <v>241</v>
+        <v>92</v>
       </c>
       <c r="H48" t="s">
         <v>82</v>
       </c>
       <c r="J48" t="s">
-        <v>242</v>
+        <v>93</v>
       </c>
       <c r="K48" t="b">
         <v>1</v>
@@ -3923,19 +3941,19 @@
         <v>84</v>
       </c>
       <c r="N48" t="s">
-        <v>162</v>
+        <v>85</v>
       </c>
       <c r="O48" t="s">
-        <v>240</v>
+        <v>80</v>
       </c>
       <c r="Q48" t="s">
-        <v>241</v>
+        <v>92</v>
       </c>
       <c r="S48" t="s">
-        <v>184</v>
+        <v>94</v>
       </c>
       <c r="T48" t="s">
-        <v>242</v>
+        <v>93</v>
       </c>
       <c r="U48" t="b">
         <v>0</v>
@@ -3946,28 +3964,19 @@
     </row>
     <row r="49" spans="1:22">
       <c r="A49" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49">
-        <v>4</v>
-      </c>
-      <c r="C49">
-        <v>5</v>
-      </c>
-      <c r="D49" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="F49" t="s">
-        <v>243</v>
+        <v>134</v>
       </c>
       <c r="G49" t="s">
-        <v>244</v>
+        <v>135</v>
       </c>
       <c r="H49" t="s">
         <v>82</v>
       </c>
       <c r="J49" t="s">
-        <v>245</v>
+        <v>136</v>
       </c>
       <c r="K49" t="b">
         <v>1</v>
@@ -3979,19 +3988,19 @@
         <v>84</v>
       </c>
       <c r="N49" t="s">
-        <v>226</v>
+        <v>137</v>
       </c>
       <c r="O49" t="s">
-        <v>243</v>
+        <v>134</v>
       </c>
       <c r="Q49" t="s">
-        <v>244</v>
+        <v>135</v>
       </c>
       <c r="S49" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="T49" t="s">
-        <v>245</v>
+        <v>136</v>
       </c>
       <c r="U49" t="b">
         <v>0</v>
@@ -4002,25 +4011,22 @@
     </row>
     <row r="50" spans="1:22">
       <c r="A50" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B50">
-        <v>4</v>
-      </c>
-      <c r="C50">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>60</v>
       </c>
       <c r="F50" t="s">
-        <v>243</v>
+        <v>166</v>
       </c>
       <c r="G50" t="s">
-        <v>246</v>
+        <v>167</v>
       </c>
       <c r="H50" t="s">
         <v>82</v>
       </c>
       <c r="J50" t="s">
-        <v>247</v>
+        <v>168</v>
       </c>
       <c r="K50" t="b">
         <v>1</v>
@@ -4032,19 +4038,19 @@
         <v>84</v>
       </c>
       <c r="N50" t="s">
-        <v>226</v>
+        <v>162</v>
       </c>
       <c r="O50" t="s">
-        <v>243</v>
+        <v>166</v>
       </c>
       <c r="Q50" t="s">
-        <v>246</v>
+        <v>167</v>
       </c>
       <c r="S50" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="T50" t="s">
-        <v>247</v>
+        <v>168</v>
       </c>
       <c r="U50" t="b">
         <v>0</v>
@@ -4055,28 +4061,22 @@
     </row>
     <row r="51" spans="1:22">
       <c r="A51" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B51">
-        <v>3</v>
-      </c>
-      <c r="C51">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D51" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F51" t="s">
-        <v>248</v>
+        <v>205</v>
       </c>
       <c r="G51" t="s">
-        <v>249</v>
+        <v>206</v>
       </c>
       <c r="H51" t="s">
         <v>82</v>
       </c>
       <c r="J51" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="K51" t="b">
         <v>1</v>
@@ -4085,22 +4085,22 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="M51" t="s">
-        <v>200</v>
+        <v>84</v>
       </c>
       <c r="N51" t="s">
-        <v>251</v>
+        <v>162</v>
       </c>
       <c r="O51" t="s">
-        <v>248</v>
+        <v>205</v>
       </c>
       <c r="Q51" t="s">
-        <v>252</v>
+        <v>206</v>
       </c>
       <c r="S51" t="s">
-        <v>86</v>
+        <v>208</v>
       </c>
       <c r="T51" t="s">
-        <v>253</v>
+        <v>207</v>
       </c>
       <c r="U51" t="b">
         <v>0</v>
@@ -4110,9 +4110,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1">
-    <sortState ref="A2:B52">
-      <sortCondition ref="A1:A52"/>
+  <autoFilter ref="A1:V1">
+    <sortState ref="A2:V51">
+      <sortCondition ref="B1:B51"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4130,7 +4130,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D62" sqref="D62:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>